<commit_message>
Agregue la hoja Noviembre
</commit_message>
<xml_diff>
--- a/Listado.xlsx
+++ b/Listado.xlsx
@@ -1,33 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Grupo Partener\Mi unidad\TUDAI\PRIMER AÑO\SEGUNDO CUATRIMESTRE\TIO\PRACTICA\TPE Git- Grupo 19\Activate-GYM\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89413E15-4686-4E00-8E68-B22F3C4D0004}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Octubre 2021" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="Noviembre 2021" sheetId="3" r:id="rId2"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="52">
   <si>
     <t>Nombre y Apellido</t>
   </si>
@@ -188,11 +188,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;\ #,##0;[Red]\-&quot;$&quot;\ #,##0"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -358,7 +358,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -410,7 +410,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -604,28 +604,28 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.42578125" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" customWidth="1"/>
     <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -648,7 +648,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -671,7 +671,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -694,7 +694,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -717,7 +717,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -740,7 +740,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -763,7 +763,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -786,7 +786,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -809,7 +809,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
@@ -832,7 +832,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
@@ -855,7 +855,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
@@ -878,7 +878,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>21</v>
       </c>
@@ -901,7 +901,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
@@ -924,7 +924,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>25</v>
       </c>
@@ -947,7 +947,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>27</v>
       </c>
@@ -970,7 +970,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>29</v>
       </c>
@@ -993,7 +993,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>30</v>
       </c>
@@ -1016,7 +1016,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>32</v>
       </c>
@@ -1039,7 +1039,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>33</v>
       </c>
@@ -1062,7 +1062,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>35</v>
       </c>
@@ -1085,7 +1085,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>51</v>
       </c>
@@ -1121,10 +1121,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F21">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F21" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Pago, Impago"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E21">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E21" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"$1200, $1800, $2300, $2700"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1134,12 +1134,534 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56D4AD6E-7CCE-4B4F-B023-AB1F8A828DA5}">
+  <dimension ref="A1:G21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>2494795241</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="2">
+        <v>1800</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2494795246</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="2">
+        <v>2700</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2494795263</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1800</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1">
+        <v>2494795208</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1200</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1">
+        <v>2494536494</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="2">
+        <v>1800</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="1">
+        <v>2494535939</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="2">
+        <v>2300</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1">
+        <v>2494480384</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="2">
+        <v>2300</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="1">
+        <v>2494485939</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="2">
+        <v>1800</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="1">
+        <v>2494481495</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="2">
+        <v>1800</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="1">
+        <v>2494485939</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="2">
+        <v>1800</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="1">
+        <v>2494478162</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="2">
+        <v>2700</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="1">
+        <v>2494556639</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="2">
+        <v>1800</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="1">
+        <v>2494546640</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="2">
+        <v>1200</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="1">
+        <v>2494624417</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="2">
+        <v>1800</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="1">
+        <v>2494628861</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="2">
+        <v>2300</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="1">
+        <v>2494628806</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" s="2">
+        <v>2300</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="1">
+        <v>2494370092</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="2">
+        <v>2700</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="1">
+        <v>2494369537</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E19" s="2">
+        <v>1800</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="1">
+        <v>2494313982</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E20" s="2">
+        <v>1200</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" s="1">
+        <v>2494013150</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E21" s="2">
+        <v>2300</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="F1:F1048576">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>"Impago"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G1:G1048576">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"NO"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E21" xr:uid="{9BAA4B1D-D5B1-456D-B328-0D1A45DE28C7}">
+      <formula1>"$1200, $1800, $2300, $2700"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F21" xr:uid="{DF7E4EA4-C374-43AB-9365-5381B0D5ADC2}">
+      <formula1>"Pago, Impago"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>